<commit_message>
Add missing lottery results and improve chart update reliability
Imports missing Daily Lottery results using direct data and improves DOM element handling for chart updates.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 7242c9e3-1c7d-4770-bc2a-a542c4aeed2f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/45399ea3-630c-4463-8e3d-edea73bb30a7/6203b99d-4ed8-49c2-b56f-81fdf11312e2.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/lottery_data_template_20250504_030312.xlsx
+++ b/attached_assets/lottery_data_template_20250504_030312.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mafor\Downloads\lottery_data_combined_20250504_030312\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80DEF1CB-5541-4875-B0DE-BBBC39E98EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE66D627-8841-4449-B35E-063A0460B734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{13E1A158-7569-4EE1-A287-820881D7B6D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3259" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3254" uniqueCount="647">
   <si>
     <t>Game Name</t>
   </si>
@@ -1965,6 +1965,18 @@
   </si>
   <si>
     <t>R3,005,678.00</t>
+  </si>
+  <si>
+    <t>R331,905.00</t>
+  </si>
+  <si>
+    <t>R276.50</t>
+  </si>
+  <si>
+    <t>R1,869,103.70</t>
+  </si>
+  <si>
+    <t>R3,729,270.00</t>
   </si>
 </sst>
 </file>
@@ -2365,7 +2377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F0C22E-4D56-4E29-9EA6-3F638E912F35}">
   <dimension ref="A1:AL151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A1:XFD8"/>
     </sheetView>
   </sheetViews>
@@ -4451,7 +4463,7 @@
         <v>43</v>
       </c>
       <c r="P20" s="3">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q20" s="3" t="s">
         <v>137</v>
@@ -10513,7 +10525,7 @@
         <v>322</v>
       </c>
       <c r="M84" s="3">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="N84" s="3" t="s">
         <v>630</v>
@@ -12718,50 +12730,50 @@
       <c r="E113" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F113" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="G113" s="5" t="s">
-        <v>123</v>
+      <c r="F113" s="3">
+        <v>2</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>643</v>
       </c>
       <c r="H113" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I113" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="J113" s="5" t="s">
-        <v>123</v>
+      <c r="I113" s="3">
+        <v>553</v>
+      </c>
+      <c r="J113" s="3" t="s">
+        <v>644</v>
       </c>
       <c r="K113" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="L113" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="M113" s="5" t="s">
-        <v>123</v>
+      <c r="L113" s="3">
+        <v>16260</v>
+      </c>
+      <c r="M113" s="3" t="s">
+        <v>565</v>
       </c>
       <c r="N113" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="O113" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="P113" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q113" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="R113" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="S113" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="T113" s="5" t="s">
-        <v>123</v>
+      <c r="O113" s="3">
+        <v>152388</v>
+      </c>
+      <c r="P113" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="Q113" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="R113" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="S113" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="T113" s="4">
+        <v>45780</v>
       </c>
     </row>
     <row r="114" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">

</xml_diff>